<commit_message>
code for api fun ,data handler
Added code
</commit_message>
<xml_diff>
--- a/src/test/resources/UserLogin.xlsx
+++ b/src/test/resources/UserLogin.xlsx
@@ -4,22 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11240" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="10560"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
     <sheet name="dietician" sheetId="2" r:id="rId2"/>
     <sheet name="patient" sheetId="3" r:id="rId3"/>
+    <sheet name="LogOutSheet" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
-  <si>
-    <t>Test</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="83">
   <si>
     <t>Scenario</t>
   </si>
@@ -30,7 +29,16 @@
     <t>password</t>
   </si>
   <si>
-    <t>Admin Login</t>
+    <t>endpoint</t>
+  </si>
+  <si>
+    <t>contentType</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>expectedCode</t>
   </si>
   <si>
     <t>valid_creds</t>
@@ -42,6 +50,15 @@
     <t>test</t>
   </si>
   <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
     <t>invalid_creds</t>
   </si>
   <si>
@@ -54,16 +71,25 @@
     <t>invalid_method</t>
   </si>
   <si>
+    <t>GET</t>
+  </si>
+  <si>
     <t>invalid_endpoint</t>
   </si>
   <si>
+    <t>/loginInvalid</t>
+  </si>
+  <si>
     <t>invalid_contentType</t>
   </si>
   <si>
-    <t>Dietician Login</t>
-  </si>
-  <si>
-    <t>Dietician01@gmail.com</t>
+    <t>application/xml</t>
+  </si>
+  <si>
+    <t>adDietician78178@gmail.com</t>
+  </si>
+  <si>
+    <t>Daffodil33</t>
   </si>
   <si>
     <t>D123@gmail.com</t>
@@ -72,15 +98,21 @@
     <t>test2</t>
   </si>
   <si>
-    <t>Patient Login</t>
-  </si>
-  <si>
-    <t>Patient01@gmail.com</t>
+    <t>adDietician63671@gmail.com</t>
+  </si>
+  <si>
+    <t>Horse77</t>
+  </si>
+  <si>
+    <t>adPatient34202@gmail.com</t>
   </si>
   <si>
     <t>@gmail.com</t>
   </si>
   <si>
+    <t>adPatient96010@gmail.com</t>
+  </si>
+  <si>
     <t>scenario</t>
   </si>
   <si>
@@ -220,6 +252,21 @@
   </si>
   <si>
     <t>1986-12-12</t>
+  </si>
+  <si>
+    <t>AdminToken</t>
+  </si>
+  <si>
+    <t>/logoutdietician</t>
+  </si>
+  <si>
+    <t>DieticianToken</t>
+  </si>
+  <si>
+    <t>PatientToken</t>
+  </si>
+  <si>
+    <t>/logoutdieticianddff</t>
   </si>
 </sst>
 </file>
@@ -232,9 +279,16 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="26">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -257,6 +311,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -264,6 +327,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -273,6 +337,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF2A00FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -406,7 +477,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,18 +486,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -560,12 +643,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,178 +788,208 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="48" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
@@ -1209,243 +1316,403 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="11.9765625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.828125" customWidth="1"/>
-    <col min="4" max="4" width="13.1484375" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="23.828125" customWidth="1"/>
+    <col min="3" max="3" width="13.1484375" customWidth="1"/>
+    <col min="4" max="4" width="10.5390625" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="7" max="7" width="13.4375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.8" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" s="5" customFormat="1" ht="15.2" spans="1:7">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" s="4" customFormat="1" ht="15" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+    </row>
+    <row r="2" s="6" customFormat="1" ht="15" spans="1:7">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" ht="14.8" spans="1:7">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="G7" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" ht="14.8" spans="1:7">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="11" ht="14.8" spans="1:7">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="12" ht="14.8" spans="1:7">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="G14">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="G15">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="Team123@gmail.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="Team3.admin@gmail.com"/>
-    <hyperlink ref="C5" r:id="rId2" display="Team3.admin@gmail.com"/>
-    <hyperlink ref="C6" r:id="rId2" display="Team3.admin@gmail.com" tooltip="mailto:Team3.admin@gmail.com"/>
-    <hyperlink ref="C7" r:id="rId3" display="Dietician01@gmail.com" tooltip="mailto:Dietician01@gmail.com"/>
-    <hyperlink ref="C8" r:id="rId4" display="D123@gmail.com" tooltip="mailto:D123@gmail.com"/>
-    <hyperlink ref="C12" r:id="rId5" display="Patient01@gmail.com" tooltip="mailto:Patient01@gmail.com"/>
-    <hyperlink ref="C10" r:id="rId3" display="Dietician01@gmail.com"/>
-    <hyperlink ref="C11" r:id="rId3" display="Dietician01@gmail.com" tooltip="mailto:Dietician01@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="Team123@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Team3.admin@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="Team3.admin@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId2" display="Team3.admin@gmail.com" tooltip="mailto:Team3.admin@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId3" display="D123@gmail.com" tooltip="mailto:D123@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId4" display="adDietician63671@gmail.com" tooltip="mailto:adDietician63671@gmail.com"/>
+    <hyperlink ref="B11" r:id="rId4" display="adDietician63671@gmail.com" tooltip="mailto:adDietician63671@gmail.com"/>
+    <hyperlink ref="B14" r:id="rId5" display="adPatient96010@gmail.com"/>
+    <hyperlink ref="B15" r:id="rId5" display="adPatient96010@gmail.com"/>
+    <hyperlink ref="B16" r:id="rId5" display="adPatient96010@gmail.com"/>
+    <hyperlink ref="B9" r:id="rId4" display="adDietician63671@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1458,7 +1725,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
@@ -1477,107 +1744,107 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>7686123101</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>33</v>
+      <c r="C2" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I2">
         <v>677976</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>7686123102</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>42</v>
+      <c r="C3" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I3">
         <v>365481</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1595,7 +1862,7 @@
   <sheetPr/>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1613,89 +1880,89 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D2">
         <v>6375480001</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>58</v>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:9">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D3">
         <v>6375480002</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>66</v>
+      <c r="E3" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1706,4 +1973,119 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="13.4375" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="13.4375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.8" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7">
+        <v>404</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>